<commit_message>
Matrix and Vertice to file
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t xml:space="preserve">Graphics Assignment No 1.</t>
   </si>
@@ -119,19 +119,82 @@
     <t xml:space="preserve">Rotation Matrix</t>
   </si>
   <si>
+    <t xml:space="preserve">0.85890	-0.40317	0.31581	0.00000
+0.44659	0.89146	-0.07650	0.00000
+-0.25069	0.20675	0.94573	0.00000
+0.00000	0.00000	0.00000	1.00000
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Image after Rotation</t>
   </si>
   <si>
+    <t xml:space="preserve">(2.0, 0.8, 0.4)
+(2.5, 2.2, 0.4)
+(1.7, 3.9, 0.8)
+(0.4, 4.4, 1.3)
+(-1.3, 3.5, 1.8)
+(1.9, -3.6, 0.1)
+(3.6, -2.7, -0.4)
+(4.1, -1.4, -0.4)
+(3.3, 0.4, 0.0)
+(1.4, 1.0, -1.4)
+(1.9, 2.3, -1.5)
+(1.1, 4.1, -1.1)
+(-0.2, 4.5, -0.6)
+(-1.9, 3.6, -0.1)
+(1.3, -3.5, -1.8)
+(3.0, -2.6, -2.3)
+(3.5, -1.3, -2.3)
+(2.7, 0.5, -1.9)
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Scale Matrix</t>
   </si>
   <si>
     <t xml:space="preserve">Single Matrix of transformations</t>
   </si>
   <si>
+    <t xml:space="preserve">2.00000	0.00000	0.00000	0.00000
+0.00000	3.00000	0.00000	0.00000
+0.00000	0.00000	4.00000	0.00000
+0.00000	0.00000	0.00000	1.00000
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Image after Scale</t>
   </si>
   <si>
+    <t xml:space="preserve">(4.1, 2.5, 1.8)
+(5.0, 6.5, 1.6)
+(3.4, 11.8, 3.3)
+(0.8, 13.1, 5.1)
+(-2.6, 10.5, 7.1)
+(3.9, -10.9, 0.5)
+(7.3, -8.2, -1.5)
+(8.2, -4.2, -1.7)
+(6.6, 1.1, -0.1)
+(2.8, 2.9, -5.8)
+(3.7, 6.9, -6.0)
+(2.1, 12.3, -4.3)
+(-0.4, 13.6, -2.5)
+(-3.9, 10.9, -0.5)
+(2.6, -10.5, -7.1)
+(6.0, -7.8, -9.1)
+(6.9, -3.8, -9.3)
+(5.3, 1.6, -7.6)
+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Translation Matrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.00000	0.00000	0.00000	4.00000
+0.00000	1.00000	0.00000	2.00000
+0.00000	0.00000	1.00000	3.00000
+0.00000	0.00000	0.00000	1.00000
+</t>
   </si>
   <si>
     <t xml:space="preserve">Image after translation</t>
@@ -230,6 +293,7 @@
       <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -631,7 +695,7 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.57"/>
@@ -848,19 +912,19 @@
   </sheetPr>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="27.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="43.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="43.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.43"/>
   </cols>
   <sheetData>
@@ -919,7 +983,9 @@
     </row>
     <row r="6" customFormat="false" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="13"/>
-      <c r="D6" s="24"/>
+      <c r="D6" s="24" t="s">
+        <v>26</v>
+      </c>
       <c r="E6" s="24"/>
       <c r="F6" s="14"/>
       <c r="G6" s="20"/>
@@ -941,7 +1007,7 @@
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C8" s="13"/>
       <c r="D8" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="25"/>
@@ -953,7 +1019,9 @@
     </row>
     <row r="9" customFormat="false" ht="124.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="13"/>
-      <c r="D9" s="24"/>
+      <c r="D9" s="24" t="s">
+        <v>28</v>
+      </c>
       <c r="E9" s="24"/>
       <c r="F9" s="25"/>
       <c r="G9" s="20"/>
@@ -975,13 +1043,13 @@
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C11" s="13"/>
       <c r="D11" s="14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" s="14"/>
       <c r="F11" s="27"/>
       <c r="G11" s="28"/>
       <c r="H11" s="29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I11" s="29"/>
       <c r="J11" s="15"/>
@@ -990,7 +1058,9 @@
     </row>
     <row r="12" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C12" s="13"/>
-      <c r="D12" s="24"/>
+      <c r="D12" s="24" t="s">
+        <v>31</v>
+      </c>
       <c r="E12" s="24"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -1016,7 +1086,7 @@
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C14" s="13"/>
       <c r="D14" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="25"/>
@@ -1030,7 +1100,9 @@
     </row>
     <row r="15" customFormat="false" ht="121.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C15" s="13"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="E15" s="24"/>
       <c r="F15" s="25"/>
       <c r="G15" s="20"/>
@@ -1056,7 +1128,7 @@
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C17" s="13"/>
       <c r="D17" s="14" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E17" s="14"/>
       <c r="F17" s="27"/>
@@ -1070,7 +1142,9 @@
     </row>
     <row r="18" customFormat="false" ht="55.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C18" s="13"/>
-      <c r="D18" s="24"/>
+      <c r="D18" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="E18" s="24"/>
       <c r="F18" s="30"/>
       <c r="H18" s="23"/>
@@ -1093,15 +1167,15 @@
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C20" s="13"/>
       <c r="D20" s="14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="25" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="29" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="I20" s="29"/>
       <c r="J20" s="25"/>
@@ -1111,7 +1185,9 @@
     </row>
     <row r="21" customFormat="false" ht="114" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C21" s="13"/>
-      <c r="D21" s="24"/>
+      <c r="D21" s="24" t="s">
+        <v>33</v>
+      </c>
       <c r="E21" s="24"/>
       <c r="F21" s="25"/>
       <c r="G21" s="25"/>
@@ -1135,7 +1211,7 @@
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C23" s="13"/>
       <c r="D23" s="14" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="32"/>
@@ -1145,7 +1221,7 @@
       <c r="J23" s="26"/>
       <c r="K23" s="27"/>
       <c r="L23" s="29" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="M23" s="29"/>
     </row>
@@ -1174,7 +1250,7 @@
       <c r="B26" s="12"/>
       <c r="C26" s="35"/>
       <c r="D26" s="29" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="20"/>
@@ -1207,12 +1283,12 @@
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="29" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="36"/>
       <c r="D29" s="14" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="32"/>
@@ -1248,18 +1324,18 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B32" s="14"/>
       <c r="C32" s="25" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="25" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
@@ -1267,7 +1343,7 @@
       <c r="J32" s="25"/>
       <c r="K32" s="25"/>
       <c r="L32" s="14" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="M32" s="14"/>
     </row>
@@ -1297,7 +1373,7 @@
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C35" s="13"/>
       <c r="D35" s="29" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="20"/>
@@ -1379,7 +1455,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Fixed issues with matrices and excel file
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects_git\ModelB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A605195-4842-4A2A-86A5-C451B323AF9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71979C58-BAE6-4AD8-BB95-6B1A350FDD89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="600" windowWidth="14400" windowHeight="15600" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
   <si>
     <t>Graphics Assignment No 1.</t>
   </si>
@@ -262,32 +262,6 @@
 (3.6, 0.2, -6.6)</t>
   </si>
   <si>
-    <t>0.00000	0.00000	0.00000	-1.00000
-0.00000	1.00000	0.00000	0.00000
-0.00000	0.00000	0.00000	-10.00000
-0.00000	0.00000	0.00000	1.00000</t>
-  </si>
-  <si>
-    <t>(0.0, 1.1, 0.0)
-(0.0, 5.1, 0.0)
-(0.0, 10.5, 0.0)
-(0.0, 11.8, 0.0)
-(0.0, 9.1, 0.0)
-(0.0, -12.3, 0.0)
-(0.0, -9.6, 0.0)
-(0.0, -5.6, 0.0)
-(0.0, -0.2, 0.0)
-(0.0, 1.6, 0.0)
-(0.0, 5.6, 0.0)
-(0.0, 10.9, 0.0)
-(0.0, 12.3, 0.0)
-(0.0, 9.6, 0.0)
-(0.0, -11.8, 0.0)
-(0.0, -9.1, 0.0)
-(0.0, -5.1, 0.0)
-(0.0, 0.2, 0.0)</t>
-  </si>
-  <si>
     <t xml:space="preserve">1.00000	0.00000	0.00000	0.00000
 0.00000	1.00000	0.00000	0.00000
 0.00000	0.00000	-1.02020	-2.02020
@@ -322,31 +296,78 @@
 (3.4, -0.6, -5.4)</t>
   </si>
   <si>
-    <t>(6.1, -10.2, 26.7)
-(4.9, -7.5, 27.4)
-(2.5, -2.1, 28.6)
-(1.3, 0.5, 29.2)
-(1.3, 0.5, 29.2)
-(10.9, -20.9, 24.3)
-(10.9, -20.9, 24.3)
-(9.7, -18.2, 24.9)
-(7.3, -12.8, 26.1)
-(-6.1, 10.2, -26.7)
-(-7.3, 12.8, -26.1)
-(-9.7, 18.2, -24.9)
-(-10.9, 20.9, -24.3)
-(-10.9, 20.9, -24.3)
-(-1.3, -0.5, -29.2)
-(-1.3, -0.5, -29.2)
-(-2.5, 2.1, -28.6)
-(-4.9, 7.5, -27.4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.00000	-1.20952	6.10845	0.00000
-0.00000	2.67439	-10.17044	0.00000
-0.00000	0.62025	26.74414	0.00000
+    <t xml:space="preserve">0.99504	0.00000	-0.09950	-1.00000
+0.00000	1.00000	0.00000	0.00000
+0.09950	0.00000	0.99504	-10.00000
+0.00000	0.00000	0.00000	1.00000
+</t>
+  </si>
+  <si>
+    <t>(2.1, 1.1, 3.0)
+(3.0, 5.1, 2.9)
+(1.2, 10.5, 4.4)
+(-1.5, 11.8, 6.0)
+(-5.1, 9.1, 7.6)
+(2.0, -12.3, 1.7)
+(5.6, -9.6, 0.0)
+(6.5, -5.6, -0.1)
+(4.8, -0.2, 1.4)
+(1.6, 1.6, -4.7)
+(2.5, 5.6, -4.7)
+(0.7, 10.9, -3.3)
+(-2.0, 12.3, -1.7)
+(-5.6, 9.6, 0.0)
+(1.5, -11.8, -6.0)
+(5.1, -9.1, -7.6)
+(6.0, -5.1, -7.7)
+(4.3, 0.2, -6.2)</t>
+  </si>
+  <si>
+    <t>(2.1, 1.1, -3.1)
+(3.0, 5.1, -3.0)
+(1.2, 10.5, -4.5)
+(-1.5, 11.8, -6.1)
+(-5.1, 9.1, -7.8)
+(2.0, -12.3, -1.7)
+(5.6, -9.6, 0.0)
+(6.5, -5.6, 0.1)
+(4.8, -0.2, -1.5)
+(1.6, 1.6, 4.7)
+(2.5, 5.6, 4.8)
+(0.7, 10.9, 3.3)
+(-2.0, 12.3, 1.7)
+(-5.6, 9.6, 0.0)
+(1.5, -11.8, 6.1)
+(5.1, -9.1, 7.8)
+(6.0, -5.1, 7.9)
+(4.3, 0.2, 6.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.83498	-1.20952	5.00044	-2.19407
+0.85829	2.67439	-9.76911	0.79470
+-0.12248	0.62025	22.85305	-7.70513
 0.00000	0.00000	-1.00000	0.00000
 </t>
+  </si>
+  <si>
+    <t>(6.8, -8.9, 22.7)
+(7.5, -5.4, 23.2)
+(5.0, 0.0, 24.5)
+(2.0, 1.8, 25.2)
+(-1.7, 0.1, 25.5)
+(8.0, -21.3, 20.5)
+(11.7, -19.6, 20.2)
+(12.3, -16.1, 20.7)
+(9.9, -10.7, 22.0)
+(-3.2, 10.6, -23.0)
+(-2.5, 14.2, -22.5)
+(-5.0, 19.5, -21.2)
+(-8.0, 21.3, -20.5)
+(-11.7, 19.6, -20.2)
+(-2.0, -1.8, -25.2)
+(1.7, -0.1, -25.5)
+(2.3, 3.5, -25.0)
+(-0.1, 8.8, -23.7)</t>
   </si>
 </sst>
 </file>
@@ -591,125 +612,125 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -797,6 +818,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1332209</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECA5D71C-C06A-4705-AFF4-A910948363A7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1828800" y="17611725"/>
+          <a:ext cx="7113884" cy="10058400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1112,98 +1188,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="K2" s="9" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="3">
         <v>123456</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="5">
         <f>MOD(C4,100)-50</f>
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="6">
         <f>INT((C4/10000))-5</f>
         <v>7</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="6">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>-1</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="6">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="7">
         <f>INT((C4/10000))-5</f>
         <v>7</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="7">
         <f>MOD(INT((C4/1000)),10)-4</f>
         <v>-1</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="7">
         <f>MOD(INT((C4/100)),10)-5</f>
         <v>-1</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="K8" s="8" t="s">
         <v>12</v>
       </c>
       <c r="L8" t="s">
@@ -1211,89 +1287,89 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="5">
         <f>MOD(C4,10)-5</f>
         <v>1</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="5">
         <f>MOD(INT((C4/10)),10)-5</f>
         <v>0</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="5">
         <f>MOD(INT((C4/100)),10)-4</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="5">
         <f>2+C7</f>
         <v>9</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="5">
         <f>3+D7</f>
         <v>2</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="5">
         <f>E7+50</f>
         <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="6">
         <f>D7</f>
         <v>-1</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="6">
         <f>C8</f>
         <v>7</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="6">
         <f>E8</f>
         <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="6">
         <f>E9</f>
         <v>0</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="6">
         <f>D7</f>
         <v>-1</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="6">
         <f>C7</f>
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1311,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24:M24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1328,529 +1404,530 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="19"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
     </row>
     <row r="3" spans="3:13" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="19"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="25"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="17"/>
     </row>
     <row r="4" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="25"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="25"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="17"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="17"/>
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="19"/>
-      <c r="D5" s="6" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="21"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="25"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="25"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="13"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="17"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" spans="3:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="19"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="25"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="25"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="17"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="17"/>
     </row>
     <row r="7" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="26"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="25"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="25"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="17"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="19"/>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="25"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="25"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="17"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="3:13" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="19"/>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="25"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="25"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="17"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="26"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="21"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="25"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="13"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="17"/>
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="19"/>
-      <c r="D11" s="6" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="3" t="s">
+      <c r="E11" s="37"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="I11" s="3"/>
-      <c r="J11" s="21"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="25"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="13"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12" spans="3:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="19"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="11"/>
+      <c r="D12" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="4" t="s">
+      <c r="E12" s="36"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="36"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="17"/>
+    </row>
+    <row r="13" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D13" s="18"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="17"/>
+    </row>
+    <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C14" s="11"/>
+      <c r="D14" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="37"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="17"/>
+    </row>
+    <row r="15" spans="3:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C15" s="11"/>
+      <c r="D15" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="17"/>
+    </row>
+    <row r="16" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="18"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="17"/>
+    </row>
+    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C17" s="11"/>
+      <c r="D17" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="17"/>
+    </row>
+    <row r="18" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="11"/>
+      <c r="D18" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="36"/>
+      <c r="F18" s="25"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="17"/>
+    </row>
+    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="18"/>
+      <c r="E19" s="19"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="17"/>
+    </row>
+    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C20" s="11"/>
+      <c r="D20" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="38"/>
+      <c r="H20" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C21" s="11"/>
+      <c r="D21" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="36"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" s="36"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="17"/>
+    </row>
+    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="18"/>
+      <c r="E22" s="19"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="13"/>
+    </row>
+    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="11"/>
+      <c r="D23" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="M23" s="35"/>
+    </row>
+    <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="11"/>
+      <c r="D24" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="25"/>
-    </row>
-    <row r="13" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="25"/>
-    </row>
-    <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="19"/>
-      <c r="D14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="25"/>
-    </row>
-    <row r="15" spans="3:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="19"/>
-      <c r="D15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="25"/>
-    </row>
-    <row r="16" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="25"/>
-    </row>
-    <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="19"/>
-      <c r="D17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="25"/>
-    </row>
-    <row r="18" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="19"/>
-      <c r="D18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="33"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="25"/>
-    </row>
-    <row r="19" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="25"/>
-    </row>
-    <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="19"/>
-      <c r="D20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="2" t="s">
+      <c r="E24" s="36"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="M24" s="36"/>
+    </row>
+    <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="18"/>
+      <c r="E25" s="19"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="25"/>
+    </row>
+    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="10"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="35"/>
+      <c r="F26" s="17"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="17"/>
+    </row>
+    <row r="27" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="36"/>
+      <c r="F27" s="17"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="17"/>
+    </row>
+    <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="30"/>
+      <c r="B28" s="27"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="19"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="17"/>
+    </row>
+    <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="37"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="17"/>
+    </row>
+    <row r="30" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="36"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="17"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="13"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="37"/>
+      <c r="C32" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="25"/>
-    </row>
-    <row r="21" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="19"/>
-      <c r="D21" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="4"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I21" s="4"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="25"/>
-    </row>
-    <row r="22" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D22" s="26"/>
-      <c r="E22" s="27"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="21"/>
-    </row>
-    <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="19"/>
-      <c r="D23" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="30"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M23" s="3"/>
-    </row>
-    <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="19"/>
-      <c r="D24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M24" s="4"/>
-    </row>
-    <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D25" s="26"/>
-      <c r="E25" s="27"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="33"/>
-    </row>
-    <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="18"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="25"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="25"/>
-    </row>
-    <row r="27" spans="1:13" ht="120" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="19"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="4"/>
-      <c r="F27" s="25"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="25"/>
-    </row>
-    <row r="28" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="38"/>
-      <c r="B28" s="35"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="25"/>
-    </row>
-    <row r="29" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="30"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="25"/>
-    </row>
-    <row r="30" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E30" s="4"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="25"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="27"/>
-      <c r="L31" s="30"/>
-      <c r="M31" s="21"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="6" t="s">
+      <c r="D32" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="D32" s="6" t="s">
+      <c r="E32" s="37"/>
+      <c r="F32" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="38"/>
+      <c r="K32" s="38"/>
+      <c r="L32" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M32" s="6"/>
+      <c r="M32" s="37"/>
     </row>
     <row r="33" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="4" t="s">
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="M33" s="4"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="M33" s="36"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27"/>
-      <c r="L34" s="34"/>
-      <c r="M34" s="34"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="26"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="L34" s="26"/>
+      <c r="M34" s="26"/>
     </row>
     <row r="35" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="19"/>
-      <c r="D35" s="3" t="s">
+      <c r="C35" s="11"/>
+      <c r="D35" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="25"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C36" s="19"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="25"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="17"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="L33:M33"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="H38:I38"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="F32:K32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>